<commit_message>
volun update and add
</commit_message>
<xml_diff>
--- a/uploads/2021_example_primary_school_Template.xlsx
+++ b/uploads/2021_example_primary_school_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lincoln Uni\Computing\639\pj2\Templates (2)\Lincoln Uni\Computing\639\Kids_uni\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lincoln Uni\Computing\639\pj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388DB76F-BB06-4835-BCD9-90A48A3D075F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BB8206-9D03-4C00-ACA6-7F444871790D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$V$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Username and passwords'!$A$6:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Username and passwords'!$A$6:$D$6</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="89">
   <si>
     <t>CU puni name (name of school or rūnanga):</t>
   </si>
@@ -50,10 +50,10 @@
     <t>CU Coordinator mobile number:</t>
   </si>
   <si>
-    <t>graduation</t>
+    <t>Grow</t>
   </si>
   <si>
-    <t>uni visit</t>
+    <t>Community Day</t>
   </si>
   <si>
     <t>Data cut-off date</t>
@@ -134,7 +134,7 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Other</t>
   </si>
   <si>
     <t>European / Pākehā</t>
@@ -143,10 +143,16 @@
     <t>Continuing</t>
   </si>
   <si>
-    <t>NZ00641</t>
+    <t>Active</t>
   </si>
   <si>
-    <t>GirlBoy</t>
+    <t>NZ100123</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
   <si>
     <t>Daisey</t>
@@ -164,7 +170,7 @@
     <t>NZ00642</t>
   </si>
   <si>
-    <t>XXX</t>
+    <t>sadfasdf</t>
   </si>
   <si>
     <t>pppppppppppppppp</t>
@@ -179,10 +185,34 @@
     <t>NZ00577</t>
   </si>
   <si>
-    <t>sadfasdf</t>
+    <t>False</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
   <si>
     <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>xl</t>
+  </si>
+  <si>
+    <t>NZ00641</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>hhhhh</t>
+  </si>
+  <si>
+    <t>NZ00688</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
   <si>
     <t>NAME</t>
@@ -236,9 +266,6 @@
     <t>MELAA (Middle Eastern, Latin American and African)</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -260,31 +287,13 @@
     <t>description</t>
   </si>
   <si>
-    <t>linconln uni</t>
+    <t>Linconln uni</t>
   </si>
   <si>
-    <t>hhhhh</t>
+    <t>ttttt</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>NZ00688</t>
-  </si>
-  <si>
-    <t>xl</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>attend</t>
+    <t>tttttt</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -565,7 +574,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -907,9 +915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X958"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:C23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -936,11 +944,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
@@ -988,11 +996,11 @@
       <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="24" t="s">
         <v>5</v>
       </c>
@@ -1014,11 +1022,11 @@
       <c r="T3" s="3"/>
     </row>
     <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="22"/>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
@@ -1044,34 +1052,34 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="W5" s="29">
-        <v>44523</v>
+        <v>44263</v>
       </c>
       <c r="X5" s="29">
-        <v>44532</v>
+        <v>44282</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,15 +1150,15 @@
         <v>32</v>
       </c>
       <c r="W6">
-        <v>10011</v>
+        <v>10013</v>
       </c>
       <c r="X6">
-        <v>10012</v>
+        <v>10014</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
-        <v>100187</v>
+        <v>100275</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>33</v>
@@ -1173,1059 +1181,956 @@
       <c r="H7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="J7" s="8">
         <v>44285</v>
       </c>
-      <c r="K7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" s="9" t="b">
-        <v>1</v>
+      <c r="K7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="O7" s="25">
-        <v>0</v>
-      </c>
-      <c r="P7" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="25">
         <v>5</v>
       </c>
-      <c r="R7" s="25">
-        <v>9</v>
-      </c>
-      <c r="S7" s="25">
-        <v>13</v>
-      </c>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
       <c r="T7" s="25"/>
-      <c r="U7" s="13"/>
+      <c r="U7" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="V7" s="13"/>
-      <c r="X7" s="21" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="8" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
-        <v>100213</v>
+        <v>100277</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E8" s="25">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="I8" s="16" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="J8" s="8">
-        <v>44285</v>
-      </c>
-      <c r="K8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8" s="9" t="b">
-        <v>1</v>
+        <v>43896</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="O8" s="25">
-        <v>20</v>
-      </c>
-      <c r="P8" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="25">
-        <v>6</v>
-      </c>
-      <c r="R8" s="25">
-        <v>10</v>
-      </c>
-      <c r="S8" s="25">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
       <c r="T8" s="25"/>
       <c r="U8" s="13"/>
-      <c r="V8" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="W8" s="21" t="s">
-        <v>85</v>
-      </c>
+      <c r="V8" s="13"/>
     </row>
     <row r="9" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25">
-        <v>100214</v>
+        <v>100279</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E9" s="25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="I9" s="16" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="J9" s="8">
-        <v>43896</v>
-      </c>
-      <c r="K9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" s="9" t="b">
-        <v>1</v>
+        <v>44285</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="O9" s="25">
-        <v>20</v>
-      </c>
-      <c r="P9" s="25">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="25">
-        <v>7</v>
-      </c>
-      <c r="R9" s="25">
-        <v>11</v>
-      </c>
-      <c r="S9" s="25">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
       <c r="T9" s="25"/>
       <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="X9" s="21" t="s">
-        <v>85</v>
+      <c r="V9" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
-        <v>100215</v>
+        <v>100280</v>
       </c>
       <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="25">
+        <v>10</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="25">
-        <v>8</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I10" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J10" s="29">
-        <v>44285</v>
-      </c>
-      <c r="K10" s="12" t="b">
+        <v>43896</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="25">
         <v>0</v>
       </c>
-      <c r="L10" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="25">
-        <v>20</v>
-      </c>
-      <c r="P10" s="25">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="25">
-        <v>8</v>
-      </c>
-      <c r="R10" s="25">
-        <v>12</v>
-      </c>
-      <c r="S10" s="25">
-        <v>16</v>
-      </c>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
       <c r="T10" s="25"/>
-      <c r="U10" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="W10" s="21" t="s">
-        <v>85</v>
+      <c r="U10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
-        <v>100216</v>
+        <v>100281</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E11" s="25">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I11" s="13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="J11" s="29">
         <v>44285</v>
       </c>
-      <c r="K11" s="12" t="b">
+      <c r="K11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="25">
         <v>0</v>
       </c>
-      <c r="L11" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="25">
-        <v>20</v>
-      </c>
-      <c r="P11" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="25">
-        <v>5</v>
-      </c>
-      <c r="R11" s="25">
-        <v>9</v>
-      </c>
-      <c r="S11" s="25">
-        <v>13</v>
-      </c>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
       <c r="T11" s="25"/>
-      <c r="V11" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="X11" s="21" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="12" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
-        <v>100217</v>
+        <v>100282</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="25">
         <v>10</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I12" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J12" s="29">
         <v>43896</v>
       </c>
-      <c r="K12" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="12" t="b">
-        <v>1</v>
+      <c r="K12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="O12" s="25">
-        <v>20</v>
-      </c>
-      <c r="P12" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="25">
-        <v>6</v>
-      </c>
-      <c r="R12" s="25">
-        <v>10</v>
-      </c>
-      <c r="S12" s="25">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
       <c r="T12" s="25"/>
-      <c r="U12" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="W12" s="21" t="s">
-        <v>85</v>
+      <c r="V12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
-        <v>100218</v>
+        <v>100283</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E13" s="25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I13" s="13" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="J13" s="29">
         <v>44285</v>
       </c>
-      <c r="K13" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="12" t="b">
-        <v>1</v>
+      <c r="K13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="O13" s="25">
-        <v>20</v>
-      </c>
-      <c r="P13" s="25">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="25">
-        <v>7</v>
-      </c>
-      <c r="R13" s="25">
-        <v>11</v>
-      </c>
-      <c r="S13" s="25">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
       <c r="T13" s="25"/>
     </row>
     <row r="14" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
-        <v>100219</v>
+        <v>100284</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E14" s="25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I14" s="13" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="J14" s="29">
-        <v>43896</v>
-      </c>
-      <c r="K14" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="12" t="b">
-        <v>1</v>
+        <v>44285</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="O14" s="25">
-        <v>20</v>
-      </c>
-      <c r="P14" s="25">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="25">
-        <v>8</v>
-      </c>
-      <c r="R14" s="25">
-        <v>12</v>
-      </c>
-      <c r="S14" s="25">
-        <v>16</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
       <c r="T14" s="25"/>
-      <c r="V14" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="X14" s="21" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="15" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
-        <v>100220</v>
+        <v>100285</v>
       </c>
       <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="25">
+        <v>10</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="25">
-        <v>8</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I15" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J15" s="29">
-        <v>44285</v>
-      </c>
-      <c r="K15" s="12" t="b">
+        <v>43896</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="25">
         <v>0</v>
       </c>
-      <c r="L15" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="25">
-        <v>20</v>
-      </c>
-      <c r="P15" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="25">
-        <v>5</v>
-      </c>
-      <c r="R15" s="25">
-        <v>9</v>
-      </c>
-      <c r="S15" s="25">
-        <v>13</v>
-      </c>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
       <c r="T15" s="25"/>
-      <c r="U15" s="26" t="s">
-        <v>82</v>
+      <c r="U15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
-        <v>100221</v>
+        <v>100286</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E16" s="25">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="H16" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I16" s="13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="J16" s="29">
         <v>44285</v>
       </c>
-      <c r="K16" s="12" t="b">
+      <c r="K16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" s="25">
         <v>0</v>
       </c>
-      <c r="L16" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="25">
-        <v>20</v>
-      </c>
-      <c r="P16" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="25">
-        <v>6</v>
-      </c>
-      <c r="R16" s="25">
-        <v>10</v>
-      </c>
-      <c r="S16" s="25">
-        <v>14</v>
-      </c>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
       <c r="T16" s="25"/>
-      <c r="W16" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25">
-        <v>100222</v>
+        <v>100287</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E17" s="25">
         <v>10</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="13"/>
+      <c r="H17" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I17" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J17" s="29">
         <v>43896</v>
       </c>
-      <c r="K17" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L17" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M17" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N17" s="12" t="b">
-        <v>1</v>
+      <c r="K17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="O17" s="25">
-        <v>20</v>
-      </c>
-      <c r="P17" s="25">
-        <v>3</v>
-      </c>
-      <c r="Q17" s="25">
-        <v>7</v>
-      </c>
-      <c r="R17" s="25">
-        <v>11</v>
-      </c>
-      <c r="S17" s="25">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
       <c r="T17" s="25"/>
-      <c r="U17" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="W17" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25">
-        <v>100223</v>
+        <v>100288</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E18" s="25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I18" s="13" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="J18" s="29">
         <v>44285</v>
       </c>
-      <c r="K18" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L18" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M18" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N18" s="12" t="b">
-        <v>1</v>
+      <c r="K18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="O18" s="25">
-        <v>20</v>
-      </c>
-      <c r="P18" s="25">
-        <v>4</v>
-      </c>
-      <c r="Q18" s="25">
+        <v>0</v>
+      </c>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <v>100289</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="25">
         <v>8</v>
       </c>
-      <c r="R18" s="25">
-        <v>12</v>
-      </c>
-      <c r="S18" s="25">
-        <v>16</v>
-      </c>
-      <c r="T18" s="25"/>
-      <c r="V18" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <v>100224</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="25">
-        <v>10</v>
-      </c>
       <c r="F19" s="13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="29">
+        <v>44285</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="O19" s="25">
+        <v>0</v>
+      </c>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+    </row>
+    <row r="20" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <v>100290</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="29">
-        <v>43896</v>
-      </c>
-      <c r="K19" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L19" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M19" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N19" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O19" s="25">
-        <v>20</v>
-      </c>
-      <c r="P19" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="25">
-        <v>5</v>
-      </c>
-      <c r="R19" s="25">
-        <v>9</v>
-      </c>
-      <c r="S19" s="25">
-        <v>13</v>
-      </c>
-      <c r="T19" s="25"/>
-    </row>
-    <row r="20" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
-        <v>100225</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="E20" s="25">
+        <v>10</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="25">
-        <v>8</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I20" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="29">
+        <v>43896</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" s="25">
+        <v>0</v>
+      </c>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <v>100291</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="29">
-        <v>44285</v>
-      </c>
-      <c r="K20" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M20" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O20" s="25">
-        <v>20</v>
-      </c>
-      <c r="P20" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="25">
-        <v>6</v>
-      </c>
-      <c r="R20" s="25">
-        <v>10</v>
-      </c>
-      <c r="S20" s="25">
-        <v>14</v>
-      </c>
-      <c r="T20" s="25"/>
-      <c r="U20" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="X20" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25">
-        <v>100226</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="E21" s="25">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="13"/>
+      <c r="H21" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I21" s="13" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="J21" s="29">
-        <v>44285</v>
-      </c>
-      <c r="K21" s="12" t="b">
+        <v>43896</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="25">
         <v>0</v>
       </c>
-      <c r="L21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O21" s="25">
-        <v>20</v>
-      </c>
-      <c r="P21" s="25">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="25">
-        <v>7</v>
-      </c>
-      <c r="R21" s="25">
-        <v>11</v>
-      </c>
-      <c r="S21" s="25">
-        <v>15</v>
-      </c>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
       <c r="T21" s="25"/>
-    </row>
-    <row r="22" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
-        <v>100227</v>
+        <v>100296</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E22" s="25">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="H22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="13"/>
       <c r="J22" s="29">
-        <v>43896</v>
-      </c>
-      <c r="K22" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L22" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M22" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N22" s="12" t="b">
-        <v>1</v>
+        <v>44285</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="O22" s="25">
-        <v>20</v>
-      </c>
-      <c r="P22" s="25">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="25">
-        <v>8</v>
-      </c>
-      <c r="R22" s="25">
+        <v>0</v>
+      </c>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
+    </row>
+    <row r="23" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <v>100297</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="25">
         <v>12</v>
-      </c>
-      <c r="S22" s="25">
-        <v>16</v>
-      </c>
-      <c r="T22" s="25"/>
-      <c r="U22" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="W22" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25">
-        <v>1</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="25">
-        <v>11</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>36</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="J23" s="31">
-        <v>43896</v>
-      </c>
-      <c r="K23" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L23" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N23" s="12" t="b">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="13"/>
+      <c r="J23" s="29">
+        <v>44285</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="O23" s="25">
         <v>0</v>
       </c>
-      <c r="P23" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="25">
-        <v>6</v>
-      </c>
-      <c r="R23" s="25">
-        <v>10</v>
-      </c>
-      <c r="S23" s="25">
-        <v>14</v>
-      </c>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
       <c r="T23" s="25"/>
-      <c r="X23" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+    </row>
+    <row r="24" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <v>100298</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="25">
+        <v>12</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="I24" s="13"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="25"/>
+      <c r="J24" s="29">
+        <v>44285</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O24" s="25">
+        <v>0</v>
+      </c>
       <c r="P24" s="25"/>
       <c r="Q24" s="25"/>
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
       <c r="T24" s="25"/>
     </row>
-    <row r="25" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
+      <c r="B25" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="E25" s="25"/>
       <c r="I25" s="13"/>
       <c r="K25" s="12"/>
@@ -2239,7 +2144,7 @@
       <c r="S25" s="25"/>
       <c r="T25" s="25"/>
     </row>
-    <row r="26" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25"/>
       <c r="E26" s="25"/>
       <c r="I26" s="13"/>
@@ -2254,7 +2159,7 @@
       <c r="S26" s="25"/>
       <c r="T26" s="25"/>
     </row>
-    <row r="27" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25"/>
       <c r="E27" s="25"/>
       <c r="I27" s="13"/>
@@ -2269,7 +2174,7 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
     </row>
-    <row r="28" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25"/>
       <c r="E28" s="25"/>
       <c r="I28" s="13"/>
@@ -2284,7 +2189,7 @@
       <c r="S28" s="25"/>
       <c r="T28" s="25"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25"/>
       <c r="E29" s="25"/>
       <c r="I29" s="13"/>
@@ -2299,7 +2204,7 @@
       <c r="S29" s="25"/>
       <c r="T29" s="25"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25"/>
       <c r="E30" s="25"/>
       <c r="I30" s="13"/>
@@ -2314,7 +2219,7 @@
       <c r="S30" s="25"/>
       <c r="T30" s="25"/>
     </row>
-    <row r="31" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25"/>
       <c r="E31" s="25"/>
       <c r="I31" s="13"/>
@@ -2329,7 +2234,7 @@
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
     </row>
-    <row r="32" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25"/>
       <c r="E32" s="25"/>
       <c r="I32" s="13"/>
@@ -15700,10 +15605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -15712,58 +15617,56 @@
     <col min="2" max="2" width="21" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="26" customWidth="1"/>
     <col min="4" max="4" width="17.3984375" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.19921875" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -15771,274 +15674,286 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>78</v>
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="1:5" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
-      <c r="E56" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:E6" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E37">
+  <autoFilter ref="A6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D37">
       <sortCondition ref="A6"/>
     </sortState>
   </autoFilter>
@@ -16061,12 +15976,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16076,42 +15991,42 @@
     </row>
     <row r="4" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -16121,27 +16036,27 @@
     </row>
     <row r="16" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17145,47 +17060,47 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10011</v>
+        <v>10013</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="31">
-        <v>44523</v>
+        <v>44263</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>10012</v>
+        <v>10014</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="31">
-        <v>44532</v>
+        <v>44282</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>